<commit_message>
Added comments, some minor code changes and some extra tests
</commit_message>
<xml_diff>
--- a/PDFDownloadTest/TestFiles/test.xlsx
+++ b/PDFDownloadTest/TestFiles/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPAC-19\source\repos\PDFDownload\PDFDownloadTest\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A0B8C7-FB7B-4583-830D-E4477254CE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05375AF7-278C-4BCD-94A1-B8E890206980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34365" yWindow="3780" windowWidth="21600" windowHeight="11235" xr2:uid="{54E64CA7-5EDF-4FCD-B7F4-52C5333015B0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54E64CA7-5EDF-4FCD-B7F4-52C5333015B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>BRnum</t>
   </si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t>Non - GRI</t>
-  </si>
-  <si>
-    <t>http://arpeissig.at/wp-content/uploads/2016/02/D7_NHB_ARP_Final_2.pdf</t>
   </si>
   <si>
     <t>http://database.globalreporting.org/reports/bfe8fd47-dc6c-ea11-a811-000d3ab11761</t>
@@ -580,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6BB547-4455-489A-812F-57EB457A5B6D}">
   <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AO2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,17 +820,14 @@
       <c r="AK2" t="s">
         <v>53</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO2" t="s">
         <v>55</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>